<commit_message>
Round settings moved to the game page
</commit_message>
<xml_diff>
--- a/Planning/csapatsorsolás.xlsx
+++ b/Planning/csapatsorsolás.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csabi\Documents\Személyes\Tanulmányok\ELTE IK\Prog Inf BsC\5.félév\Szakdolgozat\QuizProgram_LauncherConcept\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65825BE2-1588-4D8C-877E-7952B8D9CE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10477329-D8B0-4219-94A0-185CB174EA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="564" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
+    <sheet name="Munka3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="49">
   <si>
     <t>x</t>
   </si>
@@ -163,22 +164,25 @@
     <t>5,8,9,12</t>
   </si>
   <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>1,4,7,10</t>
-  </si>
-  <si>
-    <t>2,5,8,11</t>
-  </si>
-  <si>
-    <t>3,6,9,12</t>
-  </si>
-  <si>
-    <t>1,5,9,12</t>
-  </si>
-  <si>
     <t>í</t>
+  </si>
+  <si>
+    <t>5,6,7,1</t>
+  </si>
+  <si>
+    <t>2,5,3,6</t>
+  </si>
+  <si>
+    <t>4,7,2,5</t>
+  </si>
+  <si>
+    <t>körök</t>
+  </si>
+  <si>
+    <t>csapatok</t>
+  </si>
+  <si>
+    <t>körök száma:</t>
   </si>
 </sst>
 </file>
@@ -206,7 +210,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,8 +229,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -252,11 +262,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -270,11 +289,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -422,10 +476,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>411481</xdr:colOff>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>7621</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>28135</xdr:rowOff>
+      <xdr:rowOff>81475</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3053862" cy="2159053"/>
     <xdr:sp macro="" textlink="">
@@ -441,7 +495,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11509787" y="4151900"/>
+          <a:off x="12816841" y="4287715"/>
           <a:ext cx="3053862" cy="2159053"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -796,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BZ23"/>
+  <dimension ref="A1:CA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="BH9" sqref="BH9"/>
+    <sheetView topLeftCell="BI10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BN26" sqref="BN26:CO33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -823,7 +877,7 @@
     <col min="75" max="77" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -987,23 +1041,23 @@
       <c r="BT1" s="1">
         <v>7</v>
       </c>
-      <c r="BU1" s="1">
+      <c r="BU1" s="13">
         <v>8</v>
       </c>
-      <c r="BV1" s="1">
+      <c r="BV1" s="13">
         <v>9</v>
       </c>
-      <c r="BW1" s="1">
+      <c r="BW1" s="13">
         <v>10</v>
       </c>
-      <c r="BX1" s="1">
+      <c r="BX1" s="13">
         <v>11</v>
       </c>
-      <c r="BY1" s="1">
+      <c r="BY1" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1136,11 +1190,11 @@
       <c r="BN2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BO2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BP2" s="9" t="s">
-        <v>42</v>
+      <c r="BO2" s="9">
+        <v>1</v>
+      </c>
+      <c r="BP2" s="9">
+        <v>1</v>
       </c>
       <c r="BQ2" s="10">
         <v>1</v>
@@ -1148,23 +1202,19 @@
       <c r="BR2" s="10">
         <v>1</v>
       </c>
-      <c r="BS2" s="10"/>
+      <c r="BS2" s="10">
+        <v>1</v>
+      </c>
       <c r="BT2" s="10">
         <v>1</v>
       </c>
-      <c r="BU2" s="10"/>
-      <c r="BV2" s="10">
-        <v>1</v>
-      </c>
-      <c r="BW2" s="9">
-        <v>1</v>
-      </c>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="10">
-        <v>1</v>
-      </c>
+      <c r="BU2" s="14"/>
+      <c r="BV2" s="14"/>
+      <c r="BW2" s="14"/>
+      <c r="BX2" s="14"/>
+      <c r="BY2" s="14"/>
     </row>
-    <row r="3" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1287,32 +1337,34 @@
       <c r="BM3" s="8">
         <v>2</v>
       </c>
-      <c r="BN3" s="9" t="s">
-        <v>42</v>
+      <c r="BN3" s="9">
+        <v>1</v>
       </c>
       <c r="BO3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BP3" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BQ3" s="10"/>
+      <c r="BP3" s="9">
+        <v>2</v>
+      </c>
+      <c r="BQ3" s="10">
+        <v>2</v>
+      </c>
       <c r="BR3" s="10">
-        <v>1</v>
-      </c>
-      <c r="BS3" s="10"/>
-      <c r="BT3" s="10"/>
-      <c r="BU3" s="10">
-        <v>1</v>
-      </c>
-      <c r="BV3" s="9"/>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="10">
-        <v>1</v>
-      </c>
-      <c r="BY3" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="BS3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BT3" s="10">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="14"/>
+      <c r="BV3" s="14"/>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="14"/>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1433,32 +1485,32 @@
       <c r="BM4" s="8">
         <v>3</v>
       </c>
-      <c r="BN4" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BO4" s="9" t="s">
-        <v>42</v>
+      <c r="BN4" s="9">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="9">
+        <v>2</v>
       </c>
       <c r="BP4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BQ4" s="10"/>
-      <c r="BR4" s="10"/>
+      <c r="BQ4" s="10">
+        <v>1</v>
+      </c>
+      <c r="BR4" s="10">
+        <v>1</v>
+      </c>
       <c r="BS4" s="10">
         <v>1</v>
       </c>
       <c r="BT4" s="10"/>
-      <c r="BU4" s="10"/>
-      <c r="BV4" s="9">
-        <v>1</v>
-      </c>
-      <c r="BW4" s="9"/>
-      <c r="BX4" s="9"/>
-      <c r="BY4" s="9">
-        <v>1</v>
-      </c>
+      <c r="BU4" s="14"/>
+      <c r="BV4" s="14"/>
+      <c r="BW4" s="14"/>
+      <c r="BX4" s="14"/>
+      <c r="BY4" s="14"/>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1585,29 +1637,29 @@
       <c r="BN5" s="10">
         <v>1</v>
       </c>
-      <c r="BO5" s="10"/>
-      <c r="BP5" s="10"/>
+      <c r="BO5" s="10">
+        <v>2</v>
+      </c>
+      <c r="BP5" s="10">
+        <v>1</v>
+      </c>
       <c r="BQ5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BR5" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BS5" s="10" t="s">
-        <v>42</v>
-      </c>
+      <c r="BR5" s="10">
+        <v>1</v>
+      </c>
+      <c r="BS5" s="10"/>
       <c r="BT5" s="10">
         <v>1</v>
       </c>
-      <c r="BU5" s="10"/>
-      <c r="BV5" s="10"/>
-      <c r="BW5" s="10">
-        <v>1</v>
-      </c>
-      <c r="BX5" s="9"/>
-      <c r="BY5" s="9"/>
+      <c r="BU5" s="14"/>
+      <c r="BV5" s="14"/>
+      <c r="BW5" s="14"/>
+      <c r="BX5" s="14"/>
+      <c r="BY5" s="14"/>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1735,34 +1787,30 @@
         <v>1</v>
       </c>
       <c r="BO6" s="10">
-        <v>1</v>
-      </c>
-      <c r="BP6" s="10"/>
-      <c r="BQ6" s="10" t="s">
-        <v>42</v>
+        <v>2</v>
+      </c>
+      <c r="BP6" s="10">
+        <v>1</v>
+      </c>
+      <c r="BQ6" s="10">
+        <v>1</v>
       </c>
       <c r="BR6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BS6" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BT6" s="9"/>
-      <c r="BU6" s="9">
-        <v>1</v>
-      </c>
-      <c r="BV6" s="10">
-        <v>1</v>
-      </c>
-      <c r="BW6" s="9"/>
-      <c r="BX6" s="10">
-        <v>1</v>
-      </c>
-      <c r="BY6" s="10">
-        <v>1</v>
-      </c>
+      <c r="BS6" s="9">
+        <v>2</v>
+      </c>
+      <c r="BT6" s="9">
+        <v>2</v>
+      </c>
+      <c r="BU6" s="14"/>
+      <c r="BV6" s="14"/>
+      <c r="BW6" s="14"/>
+      <c r="BX6" s="14"/>
+      <c r="BY6" s="14"/>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1880,32 +1928,32 @@
       <c r="BM7" s="8">
         <v>6</v>
       </c>
-      <c r="BN7" s="10"/>
-      <c r="BO7" s="10"/>
+      <c r="BN7" s="10">
+        <v>1</v>
+      </c>
+      <c r="BO7" s="10">
+        <v>1</v>
+      </c>
       <c r="BP7" s="10">
         <v>1</v>
       </c>
-      <c r="BQ7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BR7" s="9" t="s">
-        <v>42</v>
+      <c r="BQ7" s="10"/>
+      <c r="BR7" s="9">
+        <v>2</v>
       </c>
       <c r="BS7" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BT7" s="9"/>
-      <c r="BU7" s="9"/>
-      <c r="BV7" s="9">
-        <v>1</v>
-      </c>
-      <c r="BW7" s="10"/>
-      <c r="BX7" s="10"/>
-      <c r="BY7" s="10">
-        <v>1</v>
-      </c>
+      <c r="BT7" s="9">
+        <v>1</v>
+      </c>
+      <c r="BU7" s="14"/>
+      <c r="BV7" s="14"/>
+      <c r="BW7" s="14"/>
+      <c r="BX7" s="14"/>
+      <c r="BY7" s="14"/>
     </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -2029,29 +2077,29 @@
       <c r="BN8" s="10">
         <v>1</v>
       </c>
-      <c r="BO8" s="10"/>
+      <c r="BO8" s="10">
+        <v>1</v>
+      </c>
       <c r="BP8" s="10"/>
       <c r="BQ8" s="10">
         <v>1</v>
       </c>
-      <c r="BR8" s="9"/>
-      <c r="BS8" s="9"/>
+      <c r="BR8" s="9">
+        <v>2</v>
+      </c>
+      <c r="BS8" s="9">
+        <v>1</v>
+      </c>
       <c r="BT8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="BU8" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BV8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BW8" s="10">
-        <v>1</v>
-      </c>
-      <c r="BX8" s="9"/>
-      <c r="BY8" s="9"/>
+      <c r="BU8" s="14"/>
+      <c r="BV8" s="14"/>
+      <c r="BW8" s="14"/>
+      <c r="BX8" s="14"/>
+      <c r="BY8" s="14"/>
     </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -2166,37 +2214,25 @@
         <v>2</v>
       </c>
       <c r="BH9" t="s">
-        <v>47</v>
-      </c>
-      <c r="BM9" s="8">
+        <v>42</v>
+      </c>
+      <c r="BM9" s="13">
         <v>8</v>
       </c>
-      <c r="BN9" s="10"/>
-      <c r="BO9" s="10">
-        <v>1</v>
-      </c>
-      <c r="BP9" s="10"/>
-      <c r="BQ9" s="10"/>
-      <c r="BR9" s="9">
-        <v>1</v>
-      </c>
-      <c r="BS9" s="9"/>
-      <c r="BT9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BU9" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="BV9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BW9" s="10"/>
-      <c r="BX9" s="10">
-        <v>1</v>
-      </c>
-      <c r="BY9" s="10"/>
+      <c r="BN9" s="14"/>
+      <c r="BO9" s="14"/>
+      <c r="BP9" s="14"/>
+      <c r="BQ9" s="14"/>
+      <c r="BR9" s="14"/>
+      <c r="BS9" s="14"/>
+      <c r="BT9" s="14"/>
+      <c r="BU9" s="14"/>
+      <c r="BV9" s="14"/>
+      <c r="BW9" s="14"/>
+      <c r="BX9" s="14"/>
+      <c r="BY9" s="14"/>
     </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:79" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2314,39 +2350,23 @@
       <c r="BG10" s="9">
         <v>2</v>
       </c>
-      <c r="BM10" s="8">
+      <c r="BM10" s="13">
         <v>9</v>
       </c>
-      <c r="BN10" s="10">
-        <v>1</v>
-      </c>
-      <c r="BO10" s="9"/>
-      <c r="BP10" s="9">
-        <v>1</v>
-      </c>
-      <c r="BQ10" s="10"/>
-      <c r="BR10" s="10">
-        <v>1</v>
-      </c>
-      <c r="BS10" s="9">
-        <v>1</v>
-      </c>
-      <c r="BT10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BU10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="BV10" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="BW10" s="9"/>
-      <c r="BX10" s="9"/>
-      <c r="BY10" s="9">
-        <v>2</v>
-      </c>
+      <c r="BN10" s="14"/>
+      <c r="BO10" s="14"/>
+      <c r="BP10" s="14"/>
+      <c r="BQ10" s="14"/>
+      <c r="BR10" s="14"/>
+      <c r="BS10" s="14"/>
+      <c r="BT10" s="14"/>
+      <c r="BU10" s="14"/>
+      <c r="BV10" s="14"/>
+      <c r="BW10" s="14"/>
+      <c r="BX10" s="14"/>
+      <c r="BY10" s="14"/>
     </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>0</v>
       </c>
@@ -2463,35 +2483,23 @@
       <c r="BG11" s="9">
         <v>1</v>
       </c>
-      <c r="BM11" s="8">
+      <c r="BM11" s="13">
         <v>10</v>
       </c>
-      <c r="BN11" s="9">
-        <v>1</v>
-      </c>
-      <c r="BO11" s="10"/>
-      <c r="BP11" s="9"/>
-      <c r="BQ11" s="10">
-        <v>1</v>
-      </c>
-      <c r="BR11" s="9"/>
-      <c r="BS11" s="10"/>
-      <c r="BT11" s="10">
-        <v>1</v>
-      </c>
-      <c r="BU11" s="10"/>
-      <c r="BV11" s="9"/>
-      <c r="BW11" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="BX11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BY11" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="BN11" s="14"/>
+      <c r="BO11" s="14"/>
+      <c r="BP11" s="14"/>
+      <c r="BQ11" s="14"/>
+      <c r="BR11" s="14"/>
+      <c r="BS11" s="14"/>
+      <c r="BT11" s="14"/>
+      <c r="BU11" s="14"/>
+      <c r="BV11" s="14"/>
+      <c r="BW11" s="14"/>
+      <c r="BX11" s="14"/>
+      <c r="BY11" s="14"/>
     </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>1</v>
       </c>
@@ -2596,35 +2604,23 @@
       <c r="BG12" s="9">
         <v>2</v>
       </c>
-      <c r="BM12" s="8">
+      <c r="BM12" s="13">
         <v>11</v>
       </c>
-      <c r="BN12" s="9"/>
-      <c r="BO12" s="10">
-        <v>1</v>
-      </c>
-      <c r="BP12" s="9"/>
-      <c r="BQ12" s="9"/>
-      <c r="BR12" s="10">
-        <v>1</v>
-      </c>
-      <c r="BS12" s="10"/>
-      <c r="BT12" s="9"/>
-      <c r="BU12" s="10">
-        <v>1</v>
-      </c>
-      <c r="BV12" s="10"/>
-      <c r="BW12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="BX12" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="BY12" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="BN12" s="14"/>
+      <c r="BO12" s="14"/>
+      <c r="BP12" s="14"/>
+      <c r="BQ12" s="14"/>
+      <c r="BR12" s="14"/>
+      <c r="BS12" s="14"/>
+      <c r="BT12" s="14"/>
+      <c r="BU12" s="14"/>
+      <c r="BV12" s="14"/>
+      <c r="BW12" s="14"/>
+      <c r="BX12" s="14"/>
+      <c r="BY12" s="14"/>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:79" x14ac:dyDescent="0.3">
       <c r="F13">
         <v>1</v>
       </c>
@@ -2725,35 +2721,23 @@
       <c r="BG13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="BM13" s="8">
+      <c r="BM13" s="13">
         <v>12</v>
       </c>
-      <c r="BN13" s="3"/>
-      <c r="BO13" s="3"/>
-      <c r="BP13" s="3">
-        <v>1</v>
-      </c>
-      <c r="BQ13" s="3"/>
-      <c r="BR13" s="3"/>
-      <c r="BS13" s="3">
-        <v>1</v>
-      </c>
-      <c r="BT13" s="3"/>
-      <c r="BU13" s="3"/>
-      <c r="BV13" s="3">
-        <v>1</v>
-      </c>
-      <c r="BW13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="BX13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="BY13" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="BN13" s="15"/>
+      <c r="BO13" s="15"/>
+      <c r="BP13" s="15"/>
+      <c r="BQ13" s="15"/>
+      <c r="BR13" s="15"/>
+      <c r="BS13" s="15"/>
+      <c r="BT13" s="15"/>
+      <c r="BU13" s="15"/>
+      <c r="BV13" s="15"/>
+      <c r="BW13" s="15"/>
+      <c r="BX13" s="15"/>
+      <c r="BY13" s="15"/>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2</v>
       </c>
@@ -2917,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:79" x14ac:dyDescent="0.3">
       <c r="D15">
         <v>2</v>
       </c>
@@ -2981,20 +2965,20 @@
       <c r="BN15">
         <v>1</v>
       </c>
+      <c r="BO15">
+        <v>1</v>
+      </c>
+      <c r="BP15">
+        <v>1</v>
+      </c>
       <c r="BQ15">
         <v>1</v>
       </c>
-      <c r="BT15">
-        <v>1</v>
-      </c>
-      <c r="BW15">
-        <v>1</v>
-      </c>
-      <c r="BZ15" t="s">
-        <v>43</v>
+      <c r="CA15" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:79" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>3</v>
       </c>
@@ -3055,23 +3039,23 @@
       <c r="BI16" t="s">
         <v>2</v>
       </c>
-      <c r="BO16">
-        <v>1</v>
+      <c r="BN16">
+        <v>2</v>
       </c>
       <c r="BR16">
         <v>1</v>
       </c>
-      <c r="BU16">
-        <v>1</v>
-      </c>
-      <c r="BX16">
-        <v>1</v>
-      </c>
-      <c r="BZ16" t="s">
-        <v>44</v>
+      <c r="BS16">
+        <v>1</v>
+      </c>
+      <c r="BT16">
+        <v>1</v>
+      </c>
+      <c r="CA16" t="s">
+        <v>43</v>
       </c>
     </row>
-    <row r="17" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:79" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>3</v>
       </c>
@@ -3132,23 +3116,23 @@
       <c r="BI17" t="s">
         <v>16</v>
       </c>
+      <c r="BO17">
+        <v>2</v>
+      </c>
       <c r="BP17">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="BR17">
+        <v>2</v>
       </c>
       <c r="BS17">
-        <v>1</v>
-      </c>
-      <c r="BV17">
-        <v>1</v>
-      </c>
-      <c r="BY17">
-        <v>1</v>
-      </c>
-      <c r="BZ17" t="s">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="CA17" t="s">
+        <v>44</v>
       </c>
     </row>
-    <row r="18" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:79" x14ac:dyDescent="0.3">
       <c r="E18">
         <v>3</v>
       </c>
@@ -3209,23 +3193,23 @@
       <c r="BI18" t="s">
         <v>36</v>
       </c>
-      <c r="BN18">
+      <c r="BO18">
+        <v>3</v>
+      </c>
+      <c r="BQ18">
         <v>2</v>
       </c>
       <c r="BR18">
-        <v>2</v>
-      </c>
-      <c r="BV18">
-        <v>2</v>
-      </c>
-      <c r="BY18">
-        <v>2</v>
-      </c>
-      <c r="BZ18" t="s">
-        <v>46</v>
+        <v>3</v>
+      </c>
+      <c r="BT18">
+        <v>2</v>
+      </c>
+      <c r="CA18" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="19" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:79" x14ac:dyDescent="0.3">
       <c r="P19">
         <v>2</v>
       </c>
@@ -3275,7 +3259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:79" x14ac:dyDescent="0.3">
       <c r="U20">
         <v>2</v>
       </c>
@@ -3328,7 +3312,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:79" x14ac:dyDescent="0.3">
       <c r="N21">
         <v>3</v>
       </c>
@@ -3378,7 +3362,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:79" x14ac:dyDescent="0.3">
       <c r="P22">
         <v>3</v>
       </c>
@@ -3428,7 +3412,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="3:78" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:79" x14ac:dyDescent="0.3">
       <c r="V23">
         <v>3</v>
       </c>
@@ -3628,7 +3612,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <f ca="1">NOW()</f>
-        <v>44610.974865393517</v>
+        <v>44611.578886805553</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -3650,4 +3634,924 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC3AC6D-F45D-4043-A93C-B87EB4745C8B}">
+  <dimension ref="B2:AH10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="31" width="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3" s="16">
+        <v>9</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+      <c r="O3">
+        <v>14</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3">
+        <v>17</v>
+      </c>
+      <c r="S3">
+        <v>18</v>
+      </c>
+      <c r="T3">
+        <v>19</v>
+      </c>
+      <c r="U3">
+        <v>20</v>
+      </c>
+      <c r="V3">
+        <v>21</v>
+      </c>
+      <c r="W3">
+        <v>22</v>
+      </c>
+      <c r="X3">
+        <v>23</v>
+      </c>
+      <c r="Y3">
+        <v>24</v>
+      </c>
+      <c r="Z3">
+        <v>25</v>
+      </c>
+      <c r="AA3">
+        <v>26</v>
+      </c>
+      <c r="AB3">
+        <v>27</v>
+      </c>
+      <c r="AC3">
+        <v>28</v>
+      </c>
+      <c r="AD3">
+        <v>29</v>
+      </c>
+      <c r="AE3">
+        <v>30</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>MOD($D4*E$3,$AH$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:AE10" si="0">MOD($D4*F$3,$AH$3)</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AC4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:T10" si="1">MOD($D5*E$3,$AH$3)</f>
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AE6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AC8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AE8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="16">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AE9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="16">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E4:AE10">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Shedule generation partial fix + ui changes
</commit_message>
<xml_diff>
--- a/Planning/csapatsorsolás.xlsx
+++ b/Planning/csapatsorsolás.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Csabi\Documents\Személyes\Tanulmányok\ELTE IK\Prog Inf BsC\5.félév\Szakdolgozat\QuizProgram_LauncherConcept\Planning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Szakdolgozat\Szakdolgozat\QuizProgram_LauncherConcept\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10477329-D8B0-4219-94A0-185CB174EA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E311E9E-C636-466F-BB08-9372266FE517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="564" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -297,17 +297,7 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -852,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CA23"/>
   <sheetViews>
-    <sheetView topLeftCell="BI10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BN26" sqref="BN26:CO33"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CB16" sqref="CB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3612,7 +3602,7 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <f ca="1">NOW()</f>
-        <v>44611.578886805553</v>
+        <v>44665.006664930559</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -3640,7 +3630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC3AC6D-F45D-4043-A93C-B87EB4745C8B}">
   <dimension ref="B2:AH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -4545,10 +4535,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4:AE10">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>